<commit_message>
DDT Excel config fix added
</commit_message>
<xml_diff>
--- a/src/test/java/test/testData/LoginTestData.xlsx
+++ b/src/test/java/test/testData/LoginTestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>http://test.helios2.ivt.lan/login.html</t>
   </si>
@@ -33,6 +33,18 @@
   </si>
   <si>
     <t>Vladimir Lysykh</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Логин</t>
+  </si>
+  <si>
+    <t>Пароль</t>
+  </si>
+  <si>
+    <t>Имя пользователя</t>
   </si>
   <si>
     <t>http://test3.helios2.ivt.lan/login.html</t>
@@ -51,7 +63,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,13 +81,36 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -87,15 +122,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="60% — акцент6" xfId="2" builtinId="52"/>
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -409,15 +447,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
@@ -425,22 +463,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -449,28 +487,71 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
+      <c r="A3" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
-      </c>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix MainMenu tests. Wait for Hierarchy root added
</commit_message>
<xml_diff>
--- a/src/test/java/test/testData/LoginTestData.xlsx
+++ b/src/test/java/test/testData/LoginTestData.xlsx
@@ -1,20 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\helios2_tests\src\test\java\test\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12150"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$D$4</definedName>
+  </definedNames>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,6 +24,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Логин</t>
+  </si>
+  <si>
+    <t>Пароль</t>
+  </si>
+  <si>
+    <t>Имя пользователя</t>
+  </si>
+  <si>
     <t>http://test.helios2.ivt.lan/login.html</t>
   </si>
   <si>
@@ -33,18 +43,6 @@
   </si>
   <si>
     <t>Vladimir Lysykh</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>Логин</t>
-  </si>
-  <si>
-    <t>Пароль</t>
-  </si>
-  <si>
-    <t>Имя пользователя</t>
   </si>
   <si>
     <t>http://test3.helios2.ivt.lan/login.html</t>
@@ -69,16 +67,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -96,6 +84,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -124,17 +120,17 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="60% — акцент6" xfId="2" builtinId="52"/>
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+    <cellStyle name="60% — акцент6" xfId="1" builtinId="52"/>
+    <cellStyle name="Гиперссылка" xfId="2" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -151,9 +147,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -167,7 +163,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -179,7 +175,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -191,12 +187,12 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -226,29 +222,12 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -278,26 +257,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -447,111 +409,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
+      <c r="A2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:D4"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>